<commit_message>
Updated book in wishlist
</commit_message>
<xml_diff>
--- a/data/Wishlist_nini.xlsx
+++ b/data/Wishlist_nini.xlsx
@@ -456,8 +456,16 @@
           <t>prueba</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>actualizado</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Deleted book: prueba from Nini's wishlist
</commit_message>
<xml_diff>
--- a/data/Wishlist_nini.xlsx
+++ b/data/Wishlist_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,23 +450,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>actualizado</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>aun mas mas</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added book to wishlist
</commit_message>
<xml_diff>
--- a/data/Wishlist_nini.xlsx
+++ b/data/Wishlist_nini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,15 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>prueba</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>